<commit_message>
stable pkl files used for 6-18 update to matt
</commit_message>
<xml_diff>
--- a/Candidacy-Streamlit-Repo/performance-ag-only.xlsx
+++ b/Candidacy-Streamlit-Repo/performance-ag-only.xlsx
@@ -450,28 +450,28 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>0.8263805067323644</v>
+        <v>0.7796232301019086</v>
       </c>
       <c r="D2">
-        <v>0.7883910013903975</v>
+        <v>0.7386778850941065</v>
       </c>
       <c r="E2">
-        <v>0.8630535951604434</v>
+        <v>0.8190648727158267</v>
       </c>
       <c r="F2">
-        <v>0.9370249728555917</v>
+        <v>0.9196525515743756</v>
       </c>
       <c r="G2">
-        <v>0.7157360406091371</v>
+        <v>0.6395939086294417</v>
       </c>
       <c r="H2">
-        <v>0.9390642002176278</v>
+        <v>0.9226579520697168</v>
       </c>
       <c r="I2">
-        <v>0.9370249728555917</v>
+        <v>0.9196525515743756</v>
       </c>
       <c r="J2">
-        <v>0.9380434782608695</v>
+        <v>0.921152800435019</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -482,28 +482,28 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>0.8042571250626939</v>
+        <v>0.704335389143339</v>
       </c>
       <c r="D3">
-        <v>0.7653966682008022</v>
+        <v>0.6660435680764363</v>
       </c>
       <c r="E3">
-        <v>0.8417185094358814</v>
+        <v>0.7402250480598082</v>
       </c>
       <c r="F3">
-        <v>0.9435396308360477</v>
+        <v>0.9771986970684039</v>
       </c>
       <c r="G3">
-        <v>0.6649746192893401</v>
+        <v>0.4314720812182741</v>
       </c>
       <c r="H3">
-        <v>0.9294117647058824</v>
+        <v>0.8893280632411067</v>
       </c>
       <c r="I3">
-        <v>0.9435396308360477</v>
+        <v>0.9771986970684039</v>
       </c>
       <c r="J3">
-        <v>0.9364224137931034</v>
+        <v>0.9311950336264874</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -514,28 +514,28 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>0.7340867628984165</v>
+        <v>0.7658333195544459</v>
       </c>
       <c r="D4">
-        <v>0.6961271644701137</v>
+        <v>0.7255832635751743</v>
       </c>
       <c r="E4">
-        <v>0.7706563481787226</v>
+        <v>0.8041121902961073</v>
       </c>
       <c r="F4">
-        <v>0.9554831704668838</v>
+        <v>0.9326818675352877</v>
       </c>
       <c r="G4">
-        <v>0.5126903553299492</v>
+        <v>0.5989847715736041</v>
       </c>
       <c r="H4">
-        <v>0.9016393442622951</v>
+        <v>0.9157782515991472</v>
       </c>
       <c r="I4">
-        <v>0.9554831704668838</v>
+        <v>0.9326818675352877</v>
       </c>
       <c r="J4">
-        <v>0.9277807063784924</v>
+        <v>0.9241527703066165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>